<commit_message>
adiciona novo atributo em institutição que identifica nivel do grau de estudo e perfil OPENSHIFT ao POM
</commit_message>
<xml_diff>
--- a/src/test/resources/institution.xlsx
+++ b/src/test/resources/institution.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>CODIGO</t>
   </si>
@@ -118,13 +118,19 @@
   </si>
   <si>
     <t>Fatec Taubaté</t>
+  </si>
+  <si>
+    <t>Nível</t>
+  </si>
+  <si>
+    <t>Superior</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +140,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -159,10 +173,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +494,7 @@
     <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,16 +505,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>148</v>
       </c>
@@ -510,16 +528,19 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>150</v>
       </c>
@@ -530,16 +551,19 @@
         <v>28</v>
       </c>
       <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>122</v>
       </c>
@@ -550,16 +574,19 @@
         <v>29</v>
       </c>
       <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>132</v>
       </c>
@@ -570,16 +597,19 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>164</v>
       </c>
@@ -590,16 +620,19 @@
         <v>31</v>
       </c>
       <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>189</v>
       </c>
@@ -610,16 +643,19 @@
         <v>33</v>
       </c>
       <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>212</v>
       </c>
@@ -630,12 +666,15 @@
         <v>32</v>
       </c>
       <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>